<commit_message>
Initial version of grexome_metaParse.pm, parses compatible cohorts from pathologies.xlsx
</commit_message>
<xml_diff>
--- a/Documentation/candidateGenes.xlsx
+++ b/Documentation/candidateGenes.xlsx
@@ -34,16 +34,16 @@
     <t xml:space="preserve">CFAP44</t>
   </si>
   <si>
-    <t xml:space="preserve">Flag</t>
+    <t xml:space="preserve">MMAF</t>
   </si>
   <si>
     <t xml:space="preserve">MEI1</t>
   </si>
   <si>
-    <t xml:space="preserve">Azoo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MEI4</t>
+    <t xml:space="preserve">NOA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DNAH1</t>
   </si>
   <si>
     <t xml:space="preserve">SPINK2</t>
@@ -150,10 +150,10 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
   </cols>
@@ -188,7 +188,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -196,10 +196,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
documentation for candidateGenes change: Level->Confidence score
</commit_message>
<xml_diff>
--- a/Documentation/candidateGenes.xlsx
+++ b/Documentation/candidateGenes.xlsx
@@ -22,13 +22,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
-    <t xml:space="preserve">Candidate gene</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pathology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Level</t>
+    <t xml:space="preserve">Gene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pathologyID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confidence score</t>
   </si>
   <si>
     <t xml:space="preserve">CFAP44</t>
@@ -153,9 +153,11 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>